<commit_message>
Se elimina columna con datos faltantes.
</commit_message>
<xml_diff>
--- a/Belize_Yearly.xlsx
+++ b/Belize_Yearly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maico\OneDrive - Universidad Nacional de Colombia\Oliver Pardo\VAR_VEC-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFEEA08-C790-47AD-95A9-77DC9EFBF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA60445-B78D-4BC2-821E-9EA837001C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,11 +63,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -146,7 +145,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -434,7 +433,7 @@
   <dimension ref="A1:AF27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,8 +494,8 @@
       <c r="AF1" s="6"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>2000</v>
+      <c r="A2" s="1">
+        <v>1999</v>
       </c>
       <c r="B2" s="7">
         <v>490.98024800000002</v>
@@ -507,13 +506,13 @@
       <c r="D2" s="7">
         <v>255.011696</v>
       </c>
-      <c r="E2" s="1" t="e">
+      <c r="E2" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F2" s="1" t="e">
+      <c r="F2" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="7">
         <v>2232.0175310192021</v>
       </c>
       <c r="J2" s="6"/>
@@ -542,7 +541,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B3" s="7">
         <v>713.37124700000004</v>
@@ -553,20 +552,20 @@
       <c r="D3" s="7">
         <v>386.66961400000002</v>
       </c>
-      <c r="E3" s="1" t="e">
+      <c r="E3" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F3" s="1" t="e">
+      <c r="F3" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="7">
         <v>2326.4488888011538</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B4" s="7">
         <v>526.206007</v>
@@ -577,13 +576,13 @@
       <c r="D4" s="7">
         <v>326.69704999999999</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="7">
         <v>506.086162</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="7">
         <v>350.14654300000001</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="7">
         <v>2465.5223507445717</v>
       </c>
       <c r="I4" s="3"/>
@@ -591,7 +590,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B5" s="7">
         <v>456.20044899999999</v>
@@ -602,13 +601,13 @@
       <c r="D5" s="7">
         <v>361.18086699999998</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="7">
         <v>529.51744900000006</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="7">
         <v>371.99123100000003</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="7">
         <v>2596.1885570746317</v>
       </c>
       <c r="I5" s="3"/>
@@ -616,7 +615,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B6" s="7">
         <v>491.98965900000002</v>
@@ -627,13 +626,13 @@
       <c r="D6" s="7">
         <v>396.64315900000003</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="7">
         <v>518.03733199999999</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="7">
         <v>379.91174999999998</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="7">
         <v>2779.419083707799</v>
       </c>
       <c r="I6" s="3"/>
@@ -641,7 +640,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B7" s="7">
         <v>475.45693999999997</v>
@@ -652,13 +651,13 @@
       <c r="D7" s="7">
         <v>408.248896</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="7">
         <v>547.11245799999995</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="7">
         <v>424.42378600000001</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="7">
         <v>2923.0831726157689</v>
       </c>
       <c r="I7" s="3"/>
@@ -666,7 +665,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B8" s="7">
         <v>559.90579200000002</v>
@@ -677,13 +676,13 @@
       <c r="D8" s="7">
         <v>474.74630000000002</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="7">
         <v>640.24523999999997</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="7">
         <v>493.71509700000001</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="7">
         <v>3161.9578015419029</v>
       </c>
       <c r="I8" s="3"/>
@@ -691,7 +690,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B9" s="7">
         <v>639.20798000000002</v>
@@ -702,13 +701,13 @@
       <c r="D9" s="7">
         <v>530.49083099999996</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="7">
         <v>667.90127299999995</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="7">
         <v>561.68526199999997</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="7">
         <v>3392.2307833686846</v>
       </c>
       <c r="I9" s="3"/>
@@ -716,7 +715,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B10" s="7">
         <v>790.359239</v>
@@ -727,13 +726,13 @@
       <c r="D10" s="7">
         <v>591.66249500000004</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="7">
         <v>703.23573099999999</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="7">
         <v>585.23629000000005</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="7">
         <v>3458.1869488388734</v>
       </c>
       <c r="I10" s="3"/>
@@ -741,7 +740,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B11" s="7">
         <v>784.65255400000001</v>
@@ -752,13 +751,13 @@
       <c r="D11" s="7">
         <v>594.45789300000001</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="7">
         <v>824.77648999999997</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="7">
         <v>649.59916299999998</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="7">
         <v>3361.3852888903671</v>
       </c>
       <c r="I11" s="3"/>
@@ -766,7 +765,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B12" s="7">
         <v>788.61503700000003</v>
@@ -777,13 +776,13 @@
       <c r="D12" s="7">
         <v>604.68096200000002</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="7">
         <v>859.67676100000006</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="7">
         <v>689.76021700000001</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="7">
         <v>3477.3576204725177</v>
       </c>
       <c r="I12" s="3"/>
@@ -791,7 +790,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B13" s="7">
         <v>877.53573600000004</v>
@@ -802,13 +801,13 @@
       <c r="D13" s="7">
         <v>672.36318000000006</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="7">
         <v>876.325468</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="7">
         <v>721.59071700000004</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="7">
         <v>3639.0766784993689</v>
       </c>
       <c r="I13" s="3"/>
@@ -816,7 +815,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B14" s="7">
         <v>835.66464499999995</v>
@@ -827,13 +826,13 @@
       <c r="D14" s="7">
         <v>669.86946999999998</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="7">
         <v>889.98717999999997</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="7">
         <v>729.55329400000005</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="7">
         <v>3806.4664518074901</v>
       </c>
       <c r="I14" s="3"/>
@@ -841,7 +840,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B15" s="7">
         <v>837.37576899999999</v>
@@ -852,13 +851,13 @@
       <c r="D15" s="7">
         <v>703.68514700000003</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="7">
         <v>937.857347</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="7">
         <v>777.73361699999998</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="7">
         <v>4059.1305647126392</v>
       </c>
       <c r="I15" s="3"/>
@@ -866,7 +865,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B16" s="7">
         <v>918.160347</v>
@@ -877,13 +876,13 @@
       <c r="D16" s="7">
         <v>756.51329799999996</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="7">
         <v>933.84091899999999</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="7">
         <v>778.00480100000004</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="7">
         <v>4275.9252839754372</v>
       </c>
       <c r="I16" s="3"/>
@@ -891,7 +890,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B17" s="7">
         <v>993.63645599999995</v>
@@ -902,13 +901,13 @@
       <c r="D17" s="7">
         <v>849.32772399999999</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="7">
         <v>1011.189139</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="7">
         <v>821.79164000000003</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="7">
         <v>4420.8453403863759</v>
       </c>
       <c r="I17" s="3"/>
@@ -916,7 +915,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B18" s="7">
         <v>1015.512735</v>
@@ -927,13 +926,13 @@
       <c r="D18" s="7">
         <v>864.31049399999995</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="7">
         <v>1068.2656079999999</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="7">
         <v>873.51680899999997</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="7">
         <v>4516.8601463940395</v>
       </c>
       <c r="I18" s="3"/>
@@ -941,7 +940,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B19" s="7">
         <v>1051.723534</v>
@@ -952,13 +951,13 @@
       <c r="D19" s="7">
         <v>924.67268899999999</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="7">
         <v>1151.1044220000001</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="7">
         <v>959.19295799999998</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="7">
         <v>4572.4430878851372</v>
       </c>
       <c r="I19" s="3"/>
@@ -966,7 +965,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B20" s="7">
         <v>1111.4548380000001</v>
@@ -977,13 +976,13 @@
       <c r="D20" s="7">
         <v>967.44548199999997</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="7">
         <v>1180.1031370000001</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="7">
         <v>1030.405076</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="7">
         <v>4630.0600043985105</v>
       </c>
       <c r="I20" s="3"/>
@@ -991,7 +990,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B21" s="7">
         <v>1187.972229</v>
@@ -1002,13 +1001,13 @@
       <c r="D21" s="7">
         <v>1035.3229879999999</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="7">
         <v>1208.717414</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="7">
         <v>1051.3537040000001</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="7">
         <v>4833.3014717729957</v>
       </c>
       <c r="I21" s="3"/>
@@ -1016,7 +1015,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B22" s="7">
         <v>1167.970276</v>
@@ -1027,13 +1026,13 @@
       <c r="D22" s="7">
         <v>1046.144192</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="7">
         <v>1256.208981</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="7">
         <v>1077.0008</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="7">
         <v>4160.3196740186477</v>
       </c>
       <c r="I22" s="3"/>
@@ -1041,7 +1040,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B23" s="7">
         <v>755.29012999999998</v>
@@ -1052,40 +1051,22 @@
       <c r="D23" s="7">
         <v>654.68235600000003</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="7">
         <v>1390.1060680000001</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="7">
         <v>1108.328992</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="7">
         <v>4983.3468624524012</v>
       </c>
       <c r="I23" s="3"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B24" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C24" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D24" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E24" s="4">
-        <v>1201.539587</v>
-      </c>
-      <c r="F24" s="4">
-        <v>903.17704500000002</v>
-      </c>
-      <c r="G24" s="1" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>